<commit_message>
Passage en java 7 et correction bug
</commit_message>
<xml_diff>
--- a/src/site/resources/doc/specifications/EAE-evolutions 2013.xlsx
+++ b/src/site/resources/doc/specifications/EAE-evolutions 2013.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="104">
   <si>
     <t>EAE - calcul de l'ancienneté dans le grade</t>
   </si>
@@ -545,6 +545,9 @@
   </si>
   <si>
     <t>ON FAIT QUOI PAR RAPPORT A CA ?</t>
+  </si>
+  <si>
+    <t>Vu avec Michel et la DRHFPNC, notre calcul est ok et ne doit pas tenir compte ni de l'ACC ni de la BM</t>
   </si>
 </sst>
 </file>
@@ -727,7 +730,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -928,6 +931,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,7 +1153,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1235,6 +1244,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1244,9 +1256,7 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1592,10 +1602,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:J53"/>
+  <dimension ref="B3:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,22 +1619,22 @@
     <col min="10" max="10" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="36" t="s">
+    <row r="3" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G4" s="37" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H4" s="38"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>67</v>
       </c>
@@ -1653,7 +1663,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
@@ -1673,19 +1683,20 @@
         <v>101</v>
       </c>
       <c r="J7" s="35"/>
-    </row>
-    <row r="8" spans="2:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="K7" s="40"/>
+    </row>
+    <row r="8" spans="2:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="2:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
       <c r="C9" s="12"/>
       <c r="D9" s="6"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>11</v>
       </c>
@@ -1710,7 +1721,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>91</v>
       </c>
@@ -1731,7 +1742,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
@@ -1758,7 +1769,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>62</v>
       </c>
@@ -1778,15 +1789,16 @@
         <v>93</v>
       </c>
       <c r="J13" s="28"/>
-    </row>
-    <row r="14" spans="2:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="K13" s="40"/>
+    </row>
+    <row r="14" spans="2:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="C14" s="12"/>
       <c r="D14" s="6"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="2:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>13</v>
       </c>
@@ -1813,7 +1825,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
@@ -1840,7 +1852,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>0</v>
       </c>
@@ -1861,9 +1873,11 @@
       <c r="I17" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="J17" s="28"/>
-    </row>
-    <row r="18" spans="2:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1880,8 +1894,9 @@
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
       <c r="J18" s="28"/>
-    </row>
-    <row r="19" spans="2:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="K18" s="40"/>
+    </row>
+    <row r="19" spans="2:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1901,7 +1916,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>31</v>
       </c>
@@ -1925,7 +1940,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="135" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>8</v>
       </c>
@@ -1944,8 +1959,9 @@
       </c>
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
-    </row>
-    <row r="22" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K21" s="40"/>
+    </row>
+    <row r="22" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
@@ -1967,7 +1983,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="150" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1985,7 +2001,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
@@ -2005,7 +2021,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2028,7 +2044,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>43</v>
       </c>
@@ -2038,14 +2054,14 @@
       <c r="D26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="37">
+      <c r="G26" s="38">
         <v>2</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
       <c r="J26" s="28"/>
     </row>
-    <row r="27" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>43</v>
       </c>
@@ -2055,12 +2071,12 @@
       <c r="D27" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="38"/>
+      <c r="G27" s="39"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
       <c r="J27" s="28"/>
     </row>
-    <row r="28" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>75</v>
       </c>
@@ -2075,15 +2091,15 @@
       </c>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
-      <c r="J28" s="39" t="s">
+      <c r="J28" s="36" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="31" spans="2:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="165" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>52</v>
       </c>
@@ -2104,7 +2120,7 @@
       </c>
       <c r="J31" s="28"/>
     </row>
-    <row r="32" spans="2:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="150" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Mise à jour du fichier des evolutions
</commit_message>
<xml_diff>
--- a/src/site/resources/doc/specifications/EAE-evolutions 2013.xlsx
+++ b/src/site/resources/doc/specifications/EAE-evolutions 2013.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="111">
   <si>
     <t>EAE - calcul de l'ancienneté dans le grade</t>
   </si>
@@ -548,6 +548,27 @@
   </si>
   <si>
     <t>Vu avec Michel et la DRHFPNC, notre calcul est ok et ne doit pas tenir compte ni de l'ACC ni de la BM</t>
+  </si>
+  <si>
+    <t>A voir à l'utilisation pour nous donner plus de precisions</t>
+  </si>
+  <si>
+    <t>Envoyer message erreur à SP.</t>
+  </si>
+  <si>
+    <t>On fait quelque chose dans SIRH ou on laisse la possibilité de pouvoir le faire</t>
+  </si>
+  <si>
+    <t>Si on fait l'edition en masse.</t>
+  </si>
+  <si>
+    <t>En attente reponse Titine/Fred sur impact paye.</t>
+  </si>
+  <si>
+    <t>Actuellement on peut.Par contre l'année ne sera pas rensignée.De plus l'EAE ne sera pas "finalisé" et donc ne pourra etre controlé et donc on ne recuperera rien dans les avancements. --&gt; il faut prevoir de bloquer certaines actions dans SIRH je pense. De plus, les droits ne seront pas à mis à jour sur le fichier -6&gt; ni l'agent ni son chef ne verront l'EAE dans le kiosque.</t>
+  </si>
+  <si>
+    <t>Ce WS sera appelé par SIRH lors du contrôle d'un EAE (lors du dé-contrôle on enleverra ces droits)</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1174,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1247,6 +1268,7 @@
     <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1256,7 +1278,12 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1604,8 +1631,8 @@
   </sheetPr>
   <dimension ref="B3:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="D41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,22 +1644,23 @@
     <col min="6" max="6" width="11.42578125" style="20"/>
     <col min="9" max="9" width="38" customWidth="1"/>
     <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="38"/>
+      <c r="H4" s="39"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
@@ -1683,7 +1711,7 @@
         <v>101</v>
       </c>
       <c r="J7" s="35"/>
-      <c r="K7" s="40"/>
+      <c r="K7" s="37"/>
     </row>
     <row r="8" spans="2:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="E8" s="21"/>
@@ -1789,7 +1817,7 @@
         <v>93</v>
       </c>
       <c r="J13" s="28"/>
-      <c r="K13" s="40"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="2:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
@@ -1894,7 +1922,7 @@
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
       <c r="J18" s="28"/>
-      <c r="K18" s="40"/>
+      <c r="K18" s="37"/>
     </row>
     <row r="19" spans="2:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -1959,7 +1987,7 @@
       </c>
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
-      <c r="K21" s="40"/>
+      <c r="K21" s="37"/>
     </row>
     <row r="22" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
@@ -2054,12 +2082,14 @@
       <c r="D26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="39">
         <v>2</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
+      <c r="J26" s="31" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="27" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
@@ -2071,10 +2101,12 @@
       <c r="D27" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="39"/>
+      <c r="G27" s="40"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="J27" s="31" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="28" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
@@ -2094,6 +2126,7 @@
       <c r="J28" s="36" t="s">
         <v>102</v>
       </c>
+      <c r="K28" s="37"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
@@ -2118,7 +2151,12 @@
       <c r="I31" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J31" s="28"/>
+      <c r="J31" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="K31" s="41" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="32" spans="2:11" ht="150" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
@@ -2138,8 +2176,9 @@
         <v>97</v>
       </c>
       <c r="J32" s="28"/>
-    </row>
-    <row r="33" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K32" s="37"/>
+    </row>
+    <row r="33" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>1</v>
       </c>
@@ -2155,15 +2194,18 @@
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
       <c r="J33" s="28"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="G34" s="29"/>
       <c r="H34" s="29"/>
       <c r="I34" s="29"/>
     </row>
-    <row r="35" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
@@ -2173,7 +2215,7 @@
       <c r="H35" s="30"/>
       <c r="I35" s="30"/>
     </row>
-    <row r="36" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
         <v>24</v>
       </c>
@@ -2189,8 +2231,11 @@
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
       <c r="J36" s="28"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="7"/>
@@ -2198,7 +2243,7 @@
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
     </row>
-    <row r="38" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>49</v>
       </c>
@@ -2214,8 +2259,11 @@
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
       <c r="J38" s="28"/>
-    </row>
-    <row r="40" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K38" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>3</v>
       </c>
@@ -2230,17 +2278,19 @@
       </c>
       <c r="H40" s="28"/>
       <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>57</v>
       </c>
@@ -2261,7 +2311,7 @@
       </c>
       <c r="J43" s="28"/>
     </row>
-    <row r="44" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
@@ -2278,7 +2328,7 @@
       <c r="I44" s="28"/>
       <c r="J44" s="28"/>
     </row>
-    <row r="45" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>44</v>
       </c>
@@ -2299,11 +2349,11 @@
       </c>
       <c r="J45" s="28"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="49" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>4</v>
       </c>
@@ -2321,8 +2371,11 @@
         <v>100</v>
       </c>
       <c r="J49" s="28"/>
-    </row>
-    <row r="50" spans="2:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="K49" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
@@ -2339,7 +2392,7 @@
       <c r="I50" s="28"/>
       <c r="J50" s="28"/>
     </row>
-    <row r="51" spans="2:10" ht="35.25" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" ht="35.25" x14ac:dyDescent="0.3">
       <c r="B51" s="16" t="s">
         <v>40</v>
       </c>
@@ -2356,7 +2409,7 @@
       </c>
       <c r="J51" s="28"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G53" s="32">
         <f>SUM(G7:G51)</f>
         <v>45.5</v>

</xml_diff>